<commit_message>
Validaciones de todos los textfields  y cambio de plantilla
</commit_message>
<xml_diff>
--- a/Plantilla_info_general.xlsx
+++ b/Plantilla_info_general.xlsx
@@ -7,8 +7,7 @@
     <sheet state="visible" name="H1_Muro_Eje_A" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="H1_Muro_Eje_2" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="H1_Muro_Eje_3" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="H1_Muro_Eje_4" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="H1_Piso_Cielo" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="H1_Piso_Cielo" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -16,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="105">
   <si>
     <t>PROTOCOLO
 INSPECCIÓN VISUAL DE VIVIENDAS - ACONDICIONAMIENTO AMBIENTAL</t>
@@ -1058,39 +1057,6 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1914525" cy="504825"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Imagen"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -6362,64 +6328,6 @@
     </row>
   </sheetData>
   <mergeCells count="74">
-    <mergeCell ref="G28:J28"/>
-    <mergeCell ref="G27:J27"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="G29:J29"/>
-    <mergeCell ref="G30:J30"/>
-    <mergeCell ref="C25:F27"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="G22:I23"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="M28:P28"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="P23:R23"/>
-    <mergeCell ref="M31:P31"/>
-    <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="M32:P32"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="M33:P33"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="M34:P34"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:P29"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="M30:P30"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="B7:B44"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="M27:P27"/>
-    <mergeCell ref="G25:R25"/>
-    <mergeCell ref="G26:L26"/>
-    <mergeCell ref="M26:R26"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="C6:R6"/>
-    <mergeCell ref="C7:R7"/>
-    <mergeCell ref="C8:R20"/>
     <mergeCell ref="B2:E4"/>
     <mergeCell ref="F2:N4"/>
     <mergeCell ref="O2:P2"/>
@@ -6427,851 +6335,79 @@
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="Q3:R3"/>
     <mergeCell ref="O4:P4"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="G22:I23"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="M27:P27"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="G28:J28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:P28"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:P29"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="G30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M30:P30"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="P23:R23"/>
+    <mergeCell ref="C25:F27"/>
+    <mergeCell ref="G25:R25"/>
+    <mergeCell ref="G26:L26"/>
+    <mergeCell ref="M26:R26"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="G35:R35"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="C6:R6"/>
+    <mergeCell ref="B7:B44"/>
+    <mergeCell ref="C7:R7"/>
+    <mergeCell ref="C8:R20"/>
     <mergeCell ref="P21:R21"/>
     <mergeCell ref="P22:R22"/>
-    <mergeCell ref="G35:R35"/>
     <mergeCell ref="C37:R44"/>
     <mergeCell ref="G31:J31"/>
     <mergeCell ref="K31:L31"/>
+    <mergeCell ref="M31:P31"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="C32:F32"/>
     <mergeCell ref="G32:J32"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="M32:P32"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="C33:F33"/>
     <mergeCell ref="G33:J33"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="M33:P33"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="C34:F34"/>
     <mergeCell ref="G34:J34"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="M34:P34"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="6.63"/>
-    <col customWidth="1" min="2" max="2" width="10.38"/>
-    <col customWidth="1" min="4" max="4" width="9.63"/>
-    <col customWidth="1" min="5" max="5" width="7.75"/>
-    <col customWidth="1" min="6" max="6" width="10.63"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="83"/>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="83"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="85"/>
-      <c r="B2" s="86"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="59" t="s">
-        <v>0</v>
-      </c>
-      <c r="N2" s="12"/>
-      <c r="O2" s="61"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="87"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="55"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="85"/>
-      <c r="B3" s="11"/>
-      <c r="E3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="61" t="s">
-        <v>1</v>
-      </c>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="61" t="s">
-        <v>2</v>
-      </c>
-      <c r="R3" s="9"/>
-      <c r="S3" s="55"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="85"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="74"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="74"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="55"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="83"/>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="84"/>
-      <c r="K5" s="84"/>
-      <c r="L5" s="84"/>
-      <c r="M5" s="84"/>
-      <c r="N5" s="84"/>
-      <c r="O5" s="84"/>
-      <c r="P5" s="84"/>
-      <c r="Q5" s="84"/>
-      <c r="R5" s="84"/>
-      <c r="S5" s="83"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="85"/>
-      <c r="B6" s="88" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="89" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="83"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="85"/>
-      <c r="B7" s="90">
-        <v>5.0</v>
-      </c>
-      <c r="C7" s="74"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="15"/>
-      <c r="S7" s="83"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="85"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="83"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="85"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="11"/>
-      <c r="R9" s="12"/>
-      <c r="S9" s="83"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="85"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="11"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="83"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="85"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="11"/>
-      <c r="R11" s="12"/>
-      <c r="S11" s="83"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="85"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="11"/>
-      <c r="R12" s="12"/>
-      <c r="S12" s="83"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="85"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="11"/>
-      <c r="R13" s="12"/>
-      <c r="S13" s="83"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="85"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="11"/>
-      <c r="R14" s="12"/>
-      <c r="S14" s="83"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="85"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="11"/>
-      <c r="R15" s="12"/>
-      <c r="S15" s="83"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="85"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="11"/>
-      <c r="R16" s="12"/>
-      <c r="S16" s="83"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="85"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="11"/>
-      <c r="R17" s="12"/>
-      <c r="S17" s="83"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="85"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="11"/>
-      <c r="R18" s="12"/>
-      <c r="S18" s="83"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="85"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="11"/>
-      <c r="R19" s="12"/>
-      <c r="S19" s="83"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="85"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
-      <c r="R20" s="15"/>
-      <c r="S20" s="83"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="85"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="91" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="95">
-        <v>4.0</v>
-      </c>
-      <c r="G21" s="61" t="s">
-        <v>72</v>
-      </c>
-      <c r="H21" s="28"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="60"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="29"/>
-      <c r="M21" s="61" t="s">
-        <v>73</v>
-      </c>
-      <c r="N21" s="28"/>
-      <c r="O21" s="29"/>
-      <c r="P21" s="60"/>
-      <c r="Q21" s="28"/>
-      <c r="R21" s="9"/>
-      <c r="S21" s="83"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="85"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="61" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" s="28"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="93"/>
-      <c r="G22" s="70" t="s">
-        <v>75</v>
-      </c>
-      <c r="I22" s="27"/>
-      <c r="J22" s="61" t="s">
-        <v>76</v>
-      </c>
-      <c r="K22" s="29"/>
-      <c r="L22" s="61" t="s">
-        <v>77</v>
-      </c>
-      <c r="M22" s="29"/>
-      <c r="N22" s="61" t="s">
-        <v>78</v>
-      </c>
-      <c r="O22" s="29"/>
-      <c r="P22" s="61" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q22" s="28"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="83"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="85"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="74" t="s">
-        <v>80</v>
-      </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="94"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="62"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="62"/>
-      <c r="O23" s="25"/>
-      <c r="P23" s="62"/>
-      <c r="Q23" s="13"/>
-      <c r="R23" s="15"/>
-      <c r="S23" s="83"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="85"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="57"/>
-      <c r="H24" s="57"/>
-      <c r="I24" s="57"/>
-      <c r="J24" s="57"/>
-      <c r="K24" s="57"/>
-      <c r="L24" s="57"/>
-      <c r="M24" s="57"/>
-      <c r="N24" s="57"/>
-      <c r="O24" s="57"/>
-      <c r="P24" s="57"/>
-      <c r="Q24" s="57"/>
-      <c r="R24" s="57"/>
-      <c r="S24" s="83"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="85"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="70" t="s">
-        <v>81</v>
-      </c>
-      <c r="F25" s="12"/>
-      <c r="G25" s="74" t="s">
-        <v>82</v>
-      </c>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="13"/>
-      <c r="Q25" s="13"/>
-      <c r="R25" s="15"/>
-      <c r="S25" s="83"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="85"/>
-      <c r="B26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="61" t="s">
-        <v>83</v>
-      </c>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="28"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="61" t="s">
-        <v>84</v>
-      </c>
-      <c r="N26" s="28"/>
-      <c r="O26" s="28"/>
-      <c r="P26" s="28"/>
-      <c r="Q26" s="28"/>
-      <c r="R26" s="9"/>
-      <c r="S26" s="83"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="85"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="82" t="s">
-        <v>95</v>
-      </c>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="74" t="s">
-        <v>85</v>
-      </c>
-      <c r="L27" s="15"/>
-      <c r="M27" s="82" t="s">
-        <v>95</v>
-      </c>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="74" t="s">
-        <v>85</v>
-      </c>
-      <c r="R27" s="15"/>
-      <c r="S27" s="83"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="85"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="61" t="s">
-        <v>86</v>
-      </c>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="60"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="60"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="60"/>
-      <c r="N28" s="28"/>
-      <c r="O28" s="28"/>
-      <c r="P28" s="9"/>
-      <c r="Q28" s="60"/>
-      <c r="R28" s="9"/>
-      <c r="S28" s="83"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="85"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="61" t="s">
-        <v>87</v>
-      </c>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="60"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="60"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="60"/>
-      <c r="N29" s="28"/>
-      <c r="O29" s="28"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="60"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="83"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="85"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="61" t="s">
-        <v>88</v>
-      </c>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="60"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="60"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="60"/>
-      <c r="N30" s="28"/>
-      <c r="O30" s="28"/>
-      <c r="P30" s="9"/>
-      <c r="Q30" s="60"/>
-      <c r="R30" s="9"/>
-      <c r="S30" s="83"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="85"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="61" t="s">
-        <v>89</v>
-      </c>
-      <c r="D31" s="28"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="60"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="60"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="60"/>
-      <c r="N31" s="28"/>
-      <c r="O31" s="28"/>
-      <c r="P31" s="9"/>
-      <c r="Q31" s="60"/>
-      <c r="R31" s="9"/>
-      <c r="S31" s="83"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="85"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="61" t="s">
-        <v>90</v>
-      </c>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="60"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="28"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="60"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="60"/>
-      <c r="N32" s="28"/>
-      <c r="O32" s="28"/>
-      <c r="P32" s="9"/>
-      <c r="Q32" s="60"/>
-      <c r="R32" s="9"/>
-      <c r="S32" s="83"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="85"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="61" t="s">
-        <v>91</v>
-      </c>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="60"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="60"/>
-      <c r="L33" s="9"/>
-      <c r="M33" s="60"/>
-      <c r="N33" s="28"/>
-      <c r="O33" s="28"/>
-      <c r="P33" s="9"/>
-      <c r="Q33" s="60"/>
-      <c r="R33" s="9"/>
-      <c r="S33" s="83"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="85"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="74" t="s">
-        <v>92</v>
-      </c>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="62"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="62"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="62"/>
-      <c r="N34" s="13"/>
-      <c r="O34" s="13"/>
-      <c r="P34" s="15"/>
-      <c r="Q34" s="62"/>
-      <c r="R34" s="15"/>
-      <c r="S34" s="83"/>
-    </row>
-    <row r="35">
-      <c r="A35" s="85"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="74" t="s">
-        <v>93</v>
-      </c>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="62"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
-      <c r="N35" s="13"/>
-      <c r="O35" s="13"/>
-      <c r="P35" s="13"/>
-      <c r="Q35" s="13"/>
-      <c r="R35" s="15"/>
-      <c r="S35" s="83"/>
-    </row>
-    <row r="36">
-      <c r="A36" s="85"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="57"/>
-      <c r="D36" s="57"/>
-      <c r="E36" s="57"/>
-      <c r="F36" s="57"/>
-      <c r="G36" s="57"/>
-      <c r="H36" s="57"/>
-      <c r="I36" s="57"/>
-      <c r="J36" s="57"/>
-      <c r="K36" s="57"/>
-      <c r="L36" s="57"/>
-      <c r="M36" s="57"/>
-      <c r="N36" s="57"/>
-      <c r="O36" s="57"/>
-      <c r="P36" s="57"/>
-      <c r="Q36" s="57"/>
-      <c r="R36" s="57"/>
-      <c r="S36" s="83"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="85"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="59" t="s">
-        <v>94</v>
-      </c>
-      <c r="R37" s="12"/>
-      <c r="S37" s="83"/>
-    </row>
-    <row r="38">
-      <c r="A38" s="85"/>
-      <c r="B38" s="12"/>
-      <c r="R38" s="12"/>
-      <c r="S38" s="83"/>
-    </row>
-    <row r="39">
-      <c r="A39" s="85"/>
-      <c r="B39" s="12"/>
-      <c r="R39" s="12"/>
-      <c r="S39" s="83"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="85"/>
-      <c r="B40" s="12"/>
-      <c r="R40" s="12"/>
-      <c r="S40" s="83"/>
-    </row>
-    <row r="41">
-      <c r="A41" s="85"/>
-      <c r="B41" s="12"/>
-      <c r="R41" s="12"/>
-      <c r="S41" s="83"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="85"/>
-      <c r="B42" s="12"/>
-      <c r="R42" s="12"/>
-      <c r="S42" s="83"/>
-    </row>
-    <row r="43">
-      <c r="A43" s="85"/>
-      <c r="B43" s="12"/>
-      <c r="R43" s="12"/>
-      <c r="S43" s="83"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="85"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="13"/>
-      <c r="J44" s="13"/>
-      <c r="K44" s="13"/>
-      <c r="L44" s="13"/>
-      <c r="M44" s="13"/>
-      <c r="N44" s="13"/>
-      <c r="O44" s="13"/>
-      <c r="P44" s="13"/>
-      <c r="Q44" s="13"/>
-      <c r="R44" s="15"/>
-      <c r="S44" s="83"/>
-    </row>
-    <row r="45">
-      <c r="A45" s="83"/>
-      <c r="B45" s="83"/>
-      <c r="C45" s="55"/>
-      <c r="D45" s="55"/>
-      <c r="E45" s="55"/>
-      <c r="F45" s="55"/>
-      <c r="G45" s="55"/>
-      <c r="H45" s="55"/>
-      <c r="I45" s="55"/>
-      <c r="J45" s="55"/>
-      <c r="K45" s="55"/>
-      <c r="L45" s="55"/>
-      <c r="M45" s="55"/>
-      <c r="N45" s="55"/>
-      <c r="O45" s="55"/>
-      <c r="P45" s="55"/>
-      <c r="Q45" s="55"/>
-      <c r="R45" s="55"/>
-      <c r="S45" s="83"/>
-    </row>
-  </sheetData>
-  <mergeCells count="74">
-    <mergeCell ref="M34:P34"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="G35:R35"/>
-    <mergeCell ref="C37:R44"/>
-    <mergeCell ref="G34:J34"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="G31:J31"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="G32:J32"/>
-    <mergeCell ref="G33:J33"/>
-    <mergeCell ref="M31:P31"/>
-    <mergeCell ref="M32:P32"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="M33:P33"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="M28:P28"/>
-    <mergeCell ref="M27:P27"/>
-    <mergeCell ref="G25:R25"/>
-    <mergeCell ref="G26:L26"/>
-    <mergeCell ref="M26:R26"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="C25:F27"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="B2:E4"/>
-    <mergeCell ref="G28:J28"/>
-    <mergeCell ref="G27:J27"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="G29:J29"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="B7:B44"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="M29:P29"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="P22:R22"/>
-    <mergeCell ref="M30:P30"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="G30:J30"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="C7:R7"/>
-    <mergeCell ref="C8:R20"/>
-    <mergeCell ref="F2:N4"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="G22:I23"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="P23:R23"/>
-    <mergeCell ref="C6:R6"/>
-  </mergeCells>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -8377,37 +7513,54 @@
     <mergeCell ref="L23:M23"/>
     <mergeCell ref="N23:O23"/>
     <mergeCell ref="P23:R23"/>
-    <mergeCell ref="G27:J27"/>
-    <mergeCell ref="M27:P27"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="G28:J28"/>
     <mergeCell ref="C25:F27"/>
     <mergeCell ref="G25:R25"/>
     <mergeCell ref="G26:L26"/>
     <mergeCell ref="M26:R26"/>
+    <mergeCell ref="G27:J27"/>
     <mergeCell ref="K27:L27"/>
+    <mergeCell ref="M27:P27"/>
     <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="C28:F28"/>
     <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:P28"/>
     <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="G28:J28"/>
-    <mergeCell ref="M28:P28"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="M29:P29"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="G30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="M30:P30"/>
+    <mergeCell ref="Q30:R30"/>
     <mergeCell ref="C31:F31"/>
     <mergeCell ref="G31:R31"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="G30:J30"/>
-    <mergeCell ref="M29:P29"/>
-    <mergeCell ref="M30:P30"/>
-    <mergeCell ref="G29:J29"/>
     <mergeCell ref="C52:I53"/>
     <mergeCell ref="J52:K52"/>
-    <mergeCell ref="J53:K53"/>
+    <mergeCell ref="C32:R49"/>
+    <mergeCell ref="C51:F51"/>
+    <mergeCell ref="G51:I51"/>
+    <mergeCell ref="J51:R51"/>
+    <mergeCell ref="K60:L60"/>
+    <mergeCell ref="M60:P60"/>
+    <mergeCell ref="Q60:R60"/>
+    <mergeCell ref="C61:F61"/>
+    <mergeCell ref="G61:R61"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="C6:R6"/>
+    <mergeCell ref="B7:B79"/>
+    <mergeCell ref="C7:R7"/>
+    <mergeCell ref="C8:R20"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="J21:R21"/>
+    <mergeCell ref="C62:R79"/>
     <mergeCell ref="L52:M52"/>
     <mergeCell ref="N52:O52"/>
     <mergeCell ref="P52:R52"/>
+    <mergeCell ref="J53:K53"/>
     <mergeCell ref="L53:M53"/>
     <mergeCell ref="N53:O53"/>
     <mergeCell ref="P53:R53"/>
@@ -8415,39 +7568,22 @@
     <mergeCell ref="G55:R55"/>
     <mergeCell ref="G56:L56"/>
     <mergeCell ref="M56:R56"/>
+    <mergeCell ref="G57:J57"/>
     <mergeCell ref="K57:L57"/>
+    <mergeCell ref="M57:P57"/>
     <mergeCell ref="Q57:R57"/>
     <mergeCell ref="C58:F58"/>
+    <mergeCell ref="G58:J58"/>
     <mergeCell ref="K58:L58"/>
+    <mergeCell ref="M58:P58"/>
     <mergeCell ref="Q58:R58"/>
-    <mergeCell ref="M58:P58"/>
     <mergeCell ref="C59:F59"/>
+    <mergeCell ref="G59:J59"/>
+    <mergeCell ref="K59:L59"/>
     <mergeCell ref="M59:P59"/>
-    <mergeCell ref="C62:R79"/>
-    <mergeCell ref="G58:J58"/>
-    <mergeCell ref="G60:J60"/>
-    <mergeCell ref="M60:P60"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="C6:R6"/>
-    <mergeCell ref="B7:B79"/>
-    <mergeCell ref="C7:R7"/>
-    <mergeCell ref="C8:R20"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="J21:R21"/>
-    <mergeCell ref="C32:R49"/>
-    <mergeCell ref="C51:F51"/>
-    <mergeCell ref="G51:I51"/>
-    <mergeCell ref="J51:R51"/>
-    <mergeCell ref="C61:F61"/>
-    <mergeCell ref="G61:R61"/>
-    <mergeCell ref="K59:L59"/>
     <mergeCell ref="Q59:R59"/>
     <mergeCell ref="C60:F60"/>
-    <mergeCell ref="K60:L60"/>
-    <mergeCell ref="Q60:R60"/>
-    <mergeCell ref="G59:J59"/>
-    <mergeCell ref="M57:P57"/>
-    <mergeCell ref="G57:J57"/>
+    <mergeCell ref="G60:J60"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>